<commit_message>
Update lại measurement của t
</commit_message>
<xml_diff>
--- a/Project Plan/HRM_Mesurement.xlsx
+++ b/Project Plan/HRM_Mesurement.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="209">
   <si>
     <t>No.</t>
   </si>
@@ -661,6 +661,9 @@
   </si>
   <si>
     <t>Review and update requirement process: process description</t>
+  </si>
+  <si>
+    <t>Update personal measurement information</t>
   </si>
 </sst>
 </file>
@@ -1723,11 +1726,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121425280"/>
-        <c:axId val="121525376"/>
+        <c:axId val="98739712"/>
+        <c:axId val="98741248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121425280"/>
+        <c:axId val="98739712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121525376"/>
+        <c:crossAx val="98741248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1745,7 +1748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121525376"/>
+        <c:axId val="98741248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1759,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121425280"/>
+        <c:crossAx val="98739712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1929,11 +1932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121907072"/>
-        <c:axId val="121908608"/>
+        <c:axId val="98865152"/>
+        <c:axId val="98866688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121907072"/>
+        <c:axId val="98865152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +1946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121908608"/>
+        <c:crossAx val="98866688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1951,7 +1954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121908608"/>
+        <c:axId val="98866688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,7 +1965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121907072"/>
+        <c:crossAx val="98865152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2171,11 +2174,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121987456"/>
-        <c:axId val="121988992"/>
+        <c:axId val="98801920"/>
+        <c:axId val="98803712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121987456"/>
+        <c:axId val="98801920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,7 +2188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121988992"/>
+        <c:crossAx val="98803712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2193,7 +2196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121988992"/>
+        <c:axId val="98803712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121987456"/>
+        <c:crossAx val="98801920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2413,11 +2416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122014336"/>
-        <c:axId val="122184064"/>
+        <c:axId val="99525376"/>
+        <c:axId val="99526912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122014336"/>
+        <c:axId val="99525376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,7 +2430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122184064"/>
+        <c:crossAx val="99526912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2435,7 +2438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122184064"/>
+        <c:axId val="99526912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2446,7 +2449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122014336"/>
+        <c:crossAx val="99525376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2715,11 +2718,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122267904"/>
-        <c:axId val="122269696"/>
+        <c:axId val="99283328"/>
+        <c:axId val="99284864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122267904"/>
+        <c:axId val="99283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2729,7 +2732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122269696"/>
+        <c:crossAx val="99284864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2737,7 +2740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122269696"/>
+        <c:axId val="99284864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2748,7 +2751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122267904"/>
+        <c:crossAx val="99283328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2981,11 +2984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122303616"/>
-        <c:axId val="122305152"/>
+        <c:axId val="99333632"/>
+        <c:axId val="99335168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122303616"/>
+        <c:axId val="99333632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2995,7 +2998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122305152"/>
+        <c:crossAx val="99335168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3003,7 +3006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122305152"/>
+        <c:axId val="99335168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3014,7 +3017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122303616"/>
+        <c:crossAx val="99333632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3259,11 +3262,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92669824"/>
-        <c:axId val="92671360"/>
+        <c:axId val="99414016"/>
+        <c:axId val="99415552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92669824"/>
+        <c:axId val="99414016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3273,7 +3276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92671360"/>
+        <c:crossAx val="99415552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3281,7 +3284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92671360"/>
+        <c:axId val="99415552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3292,14 +3295,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92669824"/>
+        <c:crossAx val="99414016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3849,9 +3851,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I162" sqref="I162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8028,16 +8030,28 @@
       <c r="B130" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
+      <c r="C130" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E130" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F130" s="4"/>
-      <c r="G130" s="14"/>
+      <c r="F130" s="4">
+        <v>2</v>
+      </c>
+      <c r="G130" s="14">
+        <v>40823</v>
+      </c>
       <c r="H130" s="4"/>
-      <c r="I130" s="4"/>
-      <c r="J130" s="4"/>
+      <c r="I130" s="4">
+        <v>2</v>
+      </c>
+      <c r="J130" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
@@ -8046,16 +8060,28 @@
       <c r="B131" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4"/>
+      <c r="C131" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E131" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F131" s="4"/>
-      <c r="G131" s="14"/>
+      <c r="F131" s="4">
+        <v>3</v>
+      </c>
+      <c r="G131" s="14">
+        <v>40826</v>
+      </c>
       <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
-      <c r="J131" s="4"/>
+      <c r="I131" s="4">
+        <v>2</v>
+      </c>
+      <c r="J131" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
@@ -8064,16 +8090,28 @@
       <c r="B132" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
+      <c r="C132" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E132" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F132" s="4"/>
-      <c r="G132" s="14"/>
+      <c r="F132" s="4">
+        <v>3</v>
+      </c>
+      <c r="G132" s="14">
+        <v>40829</v>
+      </c>
       <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
+      <c r="I132" s="4">
+        <v>3</v>
+      </c>
+      <c r="J132" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
@@ -8082,16 +8120,28 @@
       <c r="B133" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
+      <c r="C133" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E133" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F133" s="4"/>
-      <c r="G133" s="14"/>
+      <c r="F133" s="4">
+        <v>5</v>
+      </c>
+      <c r="G133" s="14">
+        <v>40840</v>
+      </c>
       <c r="H133" s="4"/>
-      <c r="I133" s="4"/>
-      <c r="J133" s="4"/>
+      <c r="I133" s="4">
+        <v>1</v>
+      </c>
+      <c r="J133" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
@@ -8100,16 +8150,28 @@
       <c r="B134" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
+      <c r="C134" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E134" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F134" s="4"/>
-      <c r="G134" s="14"/>
+      <c r="F134" s="4">
+        <v>5</v>
+      </c>
+      <c r="G134" s="14">
+        <v>40843</v>
+      </c>
       <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="4"/>
+      <c r="I134" s="4">
+        <v>1</v>
+      </c>
+      <c r="J134" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
@@ -8118,16 +8180,28 @@
       <c r="B135" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
+      <c r="C135" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E135" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F135" s="4"/>
-      <c r="G135" s="14"/>
+      <c r="F135" s="4">
+        <v>5</v>
+      </c>
+      <c r="G135" s="14">
+        <v>40846</v>
+      </c>
       <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
+      <c r="I135" s="4">
+        <v>2</v>
+      </c>
+      <c r="J135" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
@@ -8136,16 +8210,28 @@
       <c r="B136" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
+      <c r="C136" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E136" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F136" s="4"/>
-      <c r="G136" s="14"/>
+      <c r="F136" s="4">
+        <v>6</v>
+      </c>
+      <c r="G136" s="14">
+        <v>40847</v>
+      </c>
       <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
-      <c r="J136" s="4"/>
+      <c r="I136" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J136" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
@@ -8154,16 +8240,28 @@
       <c r="B137" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
+      <c r="C137" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E137" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F137" s="4"/>
-      <c r="G137" s="14"/>
+      <c r="F137" s="4">
+        <v>6</v>
+      </c>
+      <c r="G137" s="14">
+        <v>40852</v>
+      </c>
       <c r="H137" s="4"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="4"/>
+      <c r="I137" s="4">
+        <v>1</v>
+      </c>
+      <c r="J137" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
@@ -8172,16 +8270,28 @@
       <c r="B138" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
+      <c r="C138" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E138" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F138" s="4"/>
-      <c r="G138" s="14"/>
+      <c r="F138" s="4">
+        <v>10</v>
+      </c>
+      <c r="G138" s="14">
+        <v>40876</v>
+      </c>
       <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
+      <c r="I138" s="4">
+        <v>2</v>
+      </c>
+      <c r="J138" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
@@ -8190,16 +8300,28 @@
       <c r="B139" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
+      <c r="C139" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E139" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F139" s="4"/>
-      <c r="G139" s="14"/>
+      <c r="F139" s="4">
+        <v>11</v>
+      </c>
+      <c r="G139" s="14">
+        <v>40675</v>
+      </c>
       <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
+      <c r="I139" s="4">
+        <v>2</v>
+      </c>
+      <c r="J139" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
@@ -8208,16 +8330,28 @@
       <c r="B140" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="C140" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E140" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F140" s="4"/>
-      <c r="G140" s="14"/>
+      <c r="F140" s="4">
+        <v>7</v>
+      </c>
+      <c r="G140" s="14">
+        <v>40857</v>
+      </c>
       <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
+      <c r="I140" s="4">
+        <v>3</v>
+      </c>
+      <c r="J140" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
@@ -8226,16 +8360,28 @@
       <c r="B141" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
+      <c r="C141" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E141" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F141" s="4"/>
-      <c r="G141" s="14"/>
+      <c r="F141" s="4">
+        <v>7</v>
+      </c>
+      <c r="G141" s="14">
+        <v>40857</v>
+      </c>
       <c r="H141" s="4"/>
-      <c r="I141" s="4"/>
-      <c r="J141" s="4"/>
+      <c r="I141" s="4">
+        <v>1</v>
+      </c>
+      <c r="J141" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
@@ -8244,16 +8390,28 @@
       <c r="B142" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
+      <c r="C142" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E142" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F142" s="4"/>
-      <c r="G142" s="14"/>
+      <c r="F142" s="4">
+        <v>8</v>
+      </c>
+      <c r="G142" s="14">
+        <v>40864</v>
+      </c>
       <c r="H142" s="4"/>
-      <c r="I142" s="4"/>
-      <c r="J142" s="4"/>
+      <c r="I142" s="4">
+        <v>2</v>
+      </c>
+      <c r="J142" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
@@ -8262,16 +8420,28 @@
       <c r="B143" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
+      <c r="C143" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E143" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F143" s="4"/>
-      <c r="G143" s="14"/>
+      <c r="F143" s="4">
+        <v>8</v>
+      </c>
+      <c r="G143" s="14">
+        <v>40864</v>
+      </c>
       <c r="H143" s="4"/>
-      <c r="I143" s="4"/>
-      <c r="J143" s="4"/>
+      <c r="I143" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J143" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
@@ -8280,16 +8450,28 @@
       <c r="B144" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="C144" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E144" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F144" s="4"/>
-      <c r="G144" s="14"/>
+      <c r="F144" s="4">
+        <v>8</v>
+      </c>
+      <c r="G144" s="14">
+        <v>40867</v>
+      </c>
       <c r="H144" s="4"/>
-      <c r="I144" s="4"/>
-      <c r="J144" s="4"/>
+      <c r="I144" s="4">
+        <v>3</v>
+      </c>
+      <c r="J144" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
@@ -8298,16 +8480,28 @@
       <c r="B145" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="C145" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E145" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F145" s="4"/>
-      <c r="G145" s="14"/>
+      <c r="F145" s="4">
+        <v>9</v>
+      </c>
+      <c r="G145" s="14">
+        <v>40868</v>
+      </c>
       <c r="H145" s="4"/>
-      <c r="I145" s="4"/>
-      <c r="J145" s="4"/>
+      <c r="I145" s="4">
+        <v>1</v>
+      </c>
+      <c r="J145" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
@@ -8316,16 +8510,28 @@
       <c r="B146" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E146" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F146" s="4"/>
-      <c r="G146" s="14"/>
+      <c r="F146" s="4">
+        <v>9</v>
+      </c>
+      <c r="G146" s="14">
+        <v>40869</v>
+      </c>
       <c r="H146" s="4"/>
-      <c r="I146" s="4"/>
-      <c r="J146" s="4"/>
+      <c r="I146" s="4">
+        <v>1</v>
+      </c>
+      <c r="J146" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
@@ -8334,16 +8540,28 @@
       <c r="B147" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E147" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F147" s="4"/>
-      <c r="G147" s="14"/>
+      <c r="F147" s="4">
+        <v>9</v>
+      </c>
+      <c r="G147" s="14">
+        <v>40871</v>
+      </c>
       <c r="H147" s="4"/>
-      <c r="I147" s="4"/>
-      <c r="J147" s="4"/>
+      <c r="I147" s="4">
+        <v>5</v>
+      </c>
+      <c r="J147" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
@@ -8352,16 +8570,28 @@
       <c r="B148" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="C148" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E148" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F148" s="4"/>
-      <c r="G148" s="14"/>
+      <c r="F148" s="4">
+        <v>9</v>
+      </c>
+      <c r="G148" s="14">
+        <v>40874</v>
+      </c>
       <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
+      <c r="I148" s="4">
+        <v>2</v>
+      </c>
+      <c r="J148" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
@@ -8370,16 +8600,28 @@
       <c r="B149" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+      <c r="C149" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E149" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F149" s="4"/>
-      <c r="G149" s="14"/>
+      <c r="F149" s="4">
+        <v>10</v>
+      </c>
+      <c r="G149" s="14">
+        <v>40876</v>
+      </c>
       <c r="H149" s="4"/>
-      <c r="I149" s="4"/>
-      <c r="J149" s="4"/>
+      <c r="I149" s="4">
+        <v>1</v>
+      </c>
+      <c r="J149" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
@@ -8388,16 +8630,24 @@
       <c r="B150" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
+      <c r="C150" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E150" s="4" t="s">
         <v>176</v>
       </c>
       <c r="F150" s="4"/>
       <c r="G150" s="14"/>
       <c r="H150" s="4"/>
-      <c r="I150" s="4"/>
-      <c r="J150" s="4"/>
+      <c r="I150" s="4">
+        <v>14</v>
+      </c>
+      <c r="J150" s="4">
+        <v>50</v>
+      </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
@@ -8406,16 +8656,28 @@
       <c r="B151" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
+      <c r="C151" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E151" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F151" s="4"/>
-      <c r="G151" s="14"/>
+      <c r="F151" s="4">
+        <v>11</v>
+      </c>
+      <c r="G151" s="14">
+        <v>40883</v>
+      </c>
       <c r="H151" s="4"/>
-      <c r="I151" s="4"/>
-      <c r="J151" s="4"/>
+      <c r="I151" s="4">
+        <v>2</v>
+      </c>
+      <c r="J151" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
@@ -8424,16 +8686,28 @@
       <c r="B152" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
+      <c r="C152" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E152" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F152" s="4"/>
-      <c r="G152" s="14"/>
+      <c r="F152" s="4">
+        <v>11</v>
+      </c>
+      <c r="G152" s="14">
+        <v>40884</v>
+      </c>
       <c r="H152" s="4"/>
-      <c r="I152" s="4"/>
-      <c r="J152" s="4"/>
+      <c r="I152" s="4">
+        <v>1</v>
+      </c>
+      <c r="J152" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
@@ -8442,16 +8716,28 @@
       <c r="B153" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4"/>
+      <c r="C153" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E153" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F153" s="4"/>
-      <c r="G153" s="14"/>
+      <c r="F153" s="4">
+        <v>11</v>
+      </c>
+      <c r="G153" s="14">
+        <v>40884</v>
+      </c>
       <c r="H153" s="4"/>
-      <c r="I153" s="4"/>
-      <c r="J153" s="4"/>
+      <c r="I153" s="4">
+        <v>1</v>
+      </c>
+      <c r="J153" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
@@ -8460,16 +8746,28 @@
       <c r="B154" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4"/>
+      <c r="C154" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E154" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F154" s="4"/>
-      <c r="G154" s="14"/>
+      <c r="F154" s="4">
+        <v>11</v>
+      </c>
+      <c r="G154" s="14">
+        <v>40885</v>
+      </c>
       <c r="H154" s="4"/>
-      <c r="I154" s="4"/>
-      <c r="J154" s="4"/>
+      <c r="I154" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J154" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
@@ -8478,16 +8776,28 @@
       <c r="B155" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C155" s="4"/>
-      <c r="D155" s="4"/>
+      <c r="C155" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E155" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F155" s="4"/>
-      <c r="G155" s="14"/>
+      <c r="F155" s="4">
+        <v>11</v>
+      </c>
+      <c r="G155" s="14">
+        <v>40886</v>
+      </c>
       <c r="H155" s="4"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
+      <c r="I155" s="4">
+        <v>1</v>
+      </c>
+      <c r="J155" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
@@ -8496,16 +8806,28 @@
       <c r="B156" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C156" s="4"/>
-      <c r="D156" s="4"/>
+      <c r="C156" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E156" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F156" s="4"/>
-      <c r="G156" s="14"/>
+      <c r="F156" s="4">
+        <v>12</v>
+      </c>
+      <c r="G156" s="14">
+        <v>40888</v>
+      </c>
       <c r="H156" s="4"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="4"/>
+      <c r="I156" s="4">
+        <v>2</v>
+      </c>
+      <c r="J156" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
@@ -8514,16 +8836,28 @@
       <c r="B157" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C157" s="4"/>
-      <c r="D157" s="4"/>
+      <c r="C157" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E157" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F157" s="4"/>
-      <c r="G157" s="14"/>
+      <c r="F157" s="4">
+        <v>15</v>
+      </c>
+      <c r="G157" s="14">
+        <v>40916</v>
+      </c>
       <c r="H157" s="4"/>
-      <c r="I157" s="4"/>
-      <c r="J157" s="4"/>
+      <c r="I157" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J157" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
@@ -8532,16 +8866,28 @@
       <c r="B158" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
+      <c r="C158" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E158" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F158" s="4"/>
-      <c r="G158" s="14"/>
+      <c r="F158" s="4">
+        <v>16</v>
+      </c>
+      <c r="G158" s="14">
+        <v>40920</v>
+      </c>
       <c r="H158" s="4"/>
-      <c r="I158" s="4"/>
-      <c r="J158" s="4"/>
+      <c r="I158" s="4">
+        <v>1</v>
+      </c>
+      <c r="J158" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
@@ -8550,16 +8896,24 @@
       <c r="B159" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
+      <c r="C159" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E159" s="4" t="s">
         <v>176</v>
       </c>
       <c r="F159" s="4"/>
       <c r="G159" s="14"/>
       <c r="H159" s="4"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="4"/>
+      <c r="I159" s="4">
+        <v>4</v>
+      </c>
+      <c r="J159" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
@@ -8568,32 +8922,58 @@
       <c r="B160" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C160" s="4"/>
-      <c r="D160" s="4"/>
+      <c r="C160" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E160" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F160" s="4"/>
-      <c r="G160" s="14"/>
+      <c r="F160" s="4">
+        <v>22</v>
+      </c>
+      <c r="G160" s="14">
+        <v>40959</v>
+      </c>
       <c r="H160" s="4"/>
-      <c r="I160" s="4"/>
-      <c r="J160" s="4"/>
+      <c r="I160" s="4">
+        <v>1</v>
+      </c>
+      <c r="J160" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>161</v>
       </c>
-      <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
-      <c r="D161" s="4"/>
+      <c r="B161" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E161" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F161" s="4"/>
-      <c r="G161" s="14"/>
+      <c r="F161" s="4">
+        <v>23</v>
+      </c>
+      <c r="G161" s="14">
+        <v>40967</v>
+      </c>
       <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="4"/>
+      <c r="I161" s="4">
+        <v>1</v>
+      </c>
+      <c r="J161" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
@@ -8875,63 +9255,63 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C27 C170:C1048576 C46:C117">
-    <cfRule type="cellIs" dxfId="67" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="38" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="39" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="cellIs" dxfId="63" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="27" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="28" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="29" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C34">
-    <cfRule type="cellIs" dxfId="59" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="23" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="24" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="25" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="55" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="18" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="19" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="21" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8943,7 +9323,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:J34 J36:J45">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8955,7 +9335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J170:J174 J3:J27 J46:J103">
-    <cfRule type="colorScale" priority="223">
+    <cfRule type="colorScale" priority="225">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8967,21 +9347,21 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C126">
-    <cfRule type="cellIs" dxfId="51" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="8" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="9" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="10" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="11" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J118:J126">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8993,7 +9373,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:J117">
-    <cfRule type="colorScale" priority="303">
+    <cfRule type="colorScale" priority="305">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9005,21 +9385,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:C169">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127:J151">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J152">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J153:J161">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9679,16 +10083,16 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10918,16 +11322,16 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C34">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11668,7 +12072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C24" s="21" t="s">
         <v>4</v>
       </c>
@@ -11699,7 +12103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C25" s="21" t="s">
         <v>5</v>
       </c>
@@ -11736,16 +12140,16 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C21">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12462,7 +12866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C24" s="21" t="s">
         <v>5</v>
       </c>
@@ -12497,58 +12901,58 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="35" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C20">
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C9">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13341,7 +13745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -13374,7 +13778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -13407,7 +13811,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C27" s="21" t="s">
         <v>134</v>
       </c>
@@ -13451,7 +13855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C28" s="21" t="s">
         <v>4</v>
       </c>
@@ -13497,7 +13901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C29" s="21" t="s">
         <v>5</v>
       </c>
@@ -13549,30 +13953,30 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C25">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14303,7 +14707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C23" s="21" t="s">
         <v>4</v>
       </c>
@@ -14339,7 +14743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C24" s="21" t="s">
         <v>5</v>
       </c>
@@ -14381,16 +14785,16 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C20">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15146,7 +15550,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -15178,7 +15582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -15210,7 +15614,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C27" s="21" t="s">
         <v>134</v>
       </c>
@@ -15248,7 +15652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C28" s="21" t="s">
         <v>4</v>
       </c>
@@ -15287,7 +15691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C29" s="21" t="s">
         <v>5</v>
       </c>
@@ -15332,16 +15736,16 @@
     <sortCondition ref="F3"/>
   </sortState>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update percent actual complete
</commit_message>
<xml_diff>
--- a/Project Plan/HRM_Mesurement.xlsx
+++ b/Project Plan/HRM_Mesurement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="18195" windowHeight="8145" tabRatio="763" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="18195" windowHeight="8145" tabRatio="763" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Tung Nguyen" sheetId="7" r:id="rId7"/>
     <sheet name="Dang Nguyen" sheetId="8" r:id="rId8"/>
     <sheet name="Nguyen Dinh" sheetId="9" r:id="rId9"/>
+    <sheet name="PercentActualComplete" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Dang Nguyen'!$A$2:$J$2</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="248">
   <si>
     <t>No.</t>
   </si>
@@ -724,6 +725,64 @@
   </si>
   <si>
     <t>Programming "Subject Management"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of actual task complete per estimated
+</t>
+  </si>
+  <si>
+    <t>(Actual Finish – Start)( Plan Finish – Start) /100%</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Actual Start</t>
+  </si>
+  <si>
+    <t>Actual Finish</t>
+  </si>
+  <si>
+    <t>% work complete</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>Architect Driver</t>
+  </si>
+  <si>
+    <t>Architect Design</t>
+  </si>
+  <si>
+    <t>System test cases</t>
+  </si>
+  <si>
+    <t>Integration test cases</t>
+  </si>
+  <si>
+    <t>Acceptance test</t>
+  </si>
+  <si>
+    <t>System test</t>
+  </si>
+  <si>
+    <t>Conduct System test</t>
+  </si>
+  <si>
+    <t>Conduct Acceptance test</t>
+  </si>
+  <si>
+    <t>Conduct Integration test</t>
+  </si>
+  <si>
+    <t>Programming</t>
   </si>
 </sst>
 </file>
@@ -733,7 +792,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,6 +834,14 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -880,7 +947,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,6 +1032,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1855,11 +1924,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98755712"/>
-        <c:axId val="99494528"/>
+        <c:axId val="100009472"/>
+        <c:axId val="100011008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98755712"/>
+        <c:axId val="100009472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,7 +1938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99494528"/>
+        <c:crossAx val="100011008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1877,7 +1946,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99494528"/>
+        <c:axId val="100011008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,14 +1957,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98755712"/>
+        <c:crossAx val="100009472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2062,11 +2130,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72129920"/>
-        <c:axId val="72139904"/>
+        <c:axId val="100069376"/>
+        <c:axId val="100070912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72129920"/>
+        <c:axId val="100069376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +2144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72139904"/>
+        <c:crossAx val="100070912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2084,7 +2152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72139904"/>
+        <c:axId val="100070912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72129920"/>
+        <c:crossAx val="100069376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2304,11 +2372,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42674048"/>
-        <c:axId val="42675584"/>
+        <c:axId val="100661504"/>
+        <c:axId val="100335616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42674048"/>
+        <c:axId val="100661504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2318,7 +2386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42675584"/>
+        <c:crossAx val="100335616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2326,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42675584"/>
+        <c:axId val="100335616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,14 +2405,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42674048"/>
+        <c:crossAx val="100661504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2547,11 +2614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42738048"/>
-        <c:axId val="42739584"/>
+        <c:axId val="100389632"/>
+        <c:axId val="100391168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42738048"/>
+        <c:axId val="100389632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2561,7 +2628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42739584"/>
+        <c:crossAx val="100391168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2569,7 +2636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42739584"/>
+        <c:axId val="100391168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,14 +2647,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42738048"/>
+        <c:crossAx val="100389632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2850,11 +2916,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42764544"/>
-        <c:axId val="42774528"/>
+        <c:axId val="100487552"/>
+        <c:axId val="100489088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42764544"/>
+        <c:axId val="100487552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2864,7 +2930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42774528"/>
+        <c:crossAx val="100489088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2872,7 +2938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42774528"/>
+        <c:axId val="100489088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,14 +2949,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42764544"/>
+        <c:crossAx val="100487552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3117,11 +3182,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42845312"/>
-        <c:axId val="42846848"/>
+        <c:axId val="100514816"/>
+        <c:axId val="100729600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42845312"/>
+        <c:axId val="100514816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3131,7 +3196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42846848"/>
+        <c:crossAx val="100729600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3139,7 +3204,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42846848"/>
+        <c:axId val="100729600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3150,14 +3215,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42845312"/>
+        <c:crossAx val="100514816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3396,11 +3460,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95636480"/>
-        <c:axId val="95638272"/>
+        <c:axId val="100816384"/>
+        <c:axId val="100817920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95636480"/>
+        <c:axId val="100816384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3410,7 +3474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95638272"/>
+        <c:crossAx val="100817920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3418,7 +3482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95638272"/>
+        <c:axId val="100817920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,14 +3493,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95636480"/>
+        <c:crossAx val="100816384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3717,11 +3780,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95700480"/>
-        <c:axId val="95702016"/>
+        <c:axId val="100864000"/>
+        <c:axId val="100865536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95700480"/>
+        <c:axId val="100864000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3731,7 +3794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95702016"/>
+        <c:crossAx val="100865536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3739,7 +3802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95702016"/>
+        <c:axId val="100865536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3750,7 +3813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95700480"/>
+        <c:crossAx val="100864000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9839,6 +9902,319 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="32">
+        <v>40817</v>
+      </c>
+      <c r="C4" s="32">
+        <v>40889</v>
+      </c>
+      <c r="D4" s="32">
+        <v>40927</v>
+      </c>
+      <c r="E4" s="32">
+        <v>40929</v>
+      </c>
+      <c r="F4">
+        <f>((E4-B4)*(C4-B4))/100</f>
+        <v>80.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="32">
+        <v>40847</v>
+      </c>
+      <c r="C5" s="32">
+        <v>40905</v>
+      </c>
+      <c r="D5" s="32">
+        <v>40858</v>
+      </c>
+      <c r="E5" s="32">
+        <v>40925</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F16" si="0">((E5-B5)*(C5-B5))/100</f>
+        <v>45.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="32">
+        <v>40848</v>
+      </c>
+      <c r="C6" s="32">
+        <v>40889</v>
+      </c>
+      <c r="D6" s="32">
+        <v>40851</v>
+      </c>
+      <c r="E6" s="32">
+        <v>40928</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="32">
+        <v>40870</v>
+      </c>
+      <c r="C7" s="32">
+        <v>40906</v>
+      </c>
+      <c r="D7" s="32">
+        <v>40928</v>
+      </c>
+      <c r="E7" s="32">
+        <v>40950</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="32">
+        <v>40890</v>
+      </c>
+      <c r="C8" s="32">
+        <v>40918</v>
+      </c>
+      <c r="D8" s="32">
+        <v>40978</v>
+      </c>
+      <c r="E8" s="32">
+        <v>41016</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>35.28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="32">
+        <v>40899</v>
+      </c>
+      <c r="C9" s="32">
+        <v>41273</v>
+      </c>
+      <c r="D9" s="32">
+        <v>40950</v>
+      </c>
+      <c r="E9" s="32">
+        <v>40954</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>205.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="32">
+        <v>40910</v>
+      </c>
+      <c r="C10" s="32">
+        <v>40918</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-3272.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="32">
+        <v>40883</v>
+      </c>
+      <c r="C11" s="32">
+        <v>40891</v>
+      </c>
+      <c r="D11" s="32">
+        <v>40932</v>
+      </c>
+      <c r="E11" s="32">
+        <v>40935</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="32">
+        <v>40899</v>
+      </c>
+      <c r="C12" s="32">
+        <v>40907</v>
+      </c>
+      <c r="D12" s="32">
+        <v>40950</v>
+      </c>
+      <c r="E12" s="32">
+        <v>40954</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="32">
+        <v>40983</v>
+      </c>
+      <c r="C13" s="32">
+        <v>40984</v>
+      </c>
+      <c r="D13" s="32">
+        <v>41030</v>
+      </c>
+      <c r="E13" s="32">
+        <v>41034</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="32">
+        <v>40994</v>
+      </c>
+      <c r="C14" s="32">
+        <v>40996</v>
+      </c>
+      <c r="D14" s="32">
+        <v>41034</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-819.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="32">
+        <v>40983</v>
+      </c>
+      <c r="C15" s="32">
+        <v>40984</v>
+      </c>
+      <c r="D15" s="32">
+        <v>40974</v>
+      </c>
+      <c r="E15" s="32">
+        <v>41030</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="32">
+        <v>40875</v>
+      </c>
+      <c r="C16" s="32">
+        <v>40982</v>
+      </c>
+      <c r="D16" s="32">
+        <v>40978</v>
+      </c>
+      <c r="E16" s="32">
+        <v>41027</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>162.63999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q26"/>
@@ -17117,7 +17493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+    <sheetView topLeftCell="D22" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>

</xml_diff>